<commit_message>
add requirements and add and fix some notebooks
</commit_message>
<xml_diff>
--- a/MOOC3_Python and ML for Asset Mngt/graphical_analysis/CleanedData_Weekly.xlsx
+++ b/MOOC3_Python and ML for Asset Mngt/graphical_analysis/CleanedData_Weekly.xlsx
@@ -942,7 +942,7 @@
         <v>0.03485235846725443</v>
       </c>
       <c r="N2">
-        <v>0.06743714093111364</v>
+        <v>0.06743714093111342</v>
       </c>
       <c r="O2">
         <v>0.1153489661220319</v>
@@ -954,7 +954,7 @@
         <v>0.04256829545419727</v>
       </c>
       <c r="S2">
-        <v>0.003161193647767568</v>
+        <v>0.00316119364776779</v>
       </c>
       <c r="T2">
         <v>-0.03221824013696306</v>
@@ -1072,7 +1072,7 @@
         <v>-0.02276503557667031</v>
       </c>
       <c r="P4">
-        <v>0.01492506760943413</v>
+        <v>0.01492506760943391</v>
       </c>
       <c r="R4">
         <v>0.01795997943436345</v>
@@ -1255,7 +1255,7 @@
         <v>-0.04370567029936312</v>
       </c>
       <c r="O7">
-        <v>-0.1307246944236246</v>
+        <v>-0.1307246944236248</v>
       </c>
       <c r="P7">
         <v>-0.08126944779862055</v>
@@ -1326,7 +1326,7 @@
         <v>0.03816161416583985</v>
       </c>
       <c r="S8">
-        <v>0.005361256548489735</v>
+        <v>0.005361256548489957</v>
       </c>
       <c r="T8">
         <v>0.022989738799434</v>
@@ -1727,7 +1727,7 @@
         <v>-0.002384521436889941</v>
       </c>
       <c r="G15">
-        <v>-0.01461359369868553</v>
+        <v>-0.01461359369868565</v>
       </c>
       <c r="H15">
         <v>-0.00780174035268022</v>
@@ -1745,7 +1745,7 @@
         <v>-0.05641008598601049</v>
       </c>
       <c r="M15">
-        <v>0.05427170680434634</v>
+        <v>0.05427170680434656</v>
       </c>
       <c r="N15">
         <v>0.0615394253844328</v>
@@ -1780,7 +1780,7 @@
         <v>0.01947898765930489</v>
       </c>
       <c r="D16">
-        <v>-0.04748649868717003</v>
+        <v>-0.04748649868717014</v>
       </c>
       <c r="E16">
         <v>-0.08683045801709888</v>
@@ -1893,7 +1893,7 @@
         <v>0.06492382242706607</v>
       </c>
       <c r="X17">
-        <v>0.05748427637527342</v>
+        <v>0.05748427637527365</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -1999,7 +1999,7 @@
         <v>0.05934841405675106</v>
       </c>
       <c r="O19">
-        <v>-0.003596647668620445</v>
+        <v>-0.003596647668620667</v>
       </c>
       <c r="P19">
         <v>0.029767505094352</v>
@@ -2223,13 +2223,13 @@
         <v>0.1267772332490622</v>
       </c>
       <c r="G23">
-        <v>0.1373389335806994</v>
+        <v>0.1373389335806996</v>
       </c>
       <c r="H23">
         <v>0.06370117244416607</v>
       </c>
       <c r="I23">
-        <v>0.07605772750163742</v>
+        <v>0.07605772750163764</v>
       </c>
       <c r="J23">
         <v>0.2444050126884956</v>
@@ -2468,10 +2468,10 @@
         <v>-0.01073789194268604</v>
       </c>
       <c r="F27">
-        <v>-0.09234932244298477</v>
+        <v>-0.09234932244298466</v>
       </c>
       <c r="G27">
-        <v>-0.02626262577046667</v>
+        <v>-0.02626262577046679</v>
       </c>
       <c r="H27">
         <v>0.01472374996068093</v>
@@ -2566,13 +2566,13 @@
         <v>-0.01031631996021443</v>
       </c>
       <c r="S28">
-        <v>-0.02099572058385846</v>
+        <v>-0.02099572058385824</v>
       </c>
       <c r="T28">
         <v>0.03937930232842679</v>
       </c>
       <c r="V28">
-        <v>0.0249996263555563</v>
+        <v>0.02499962635555608</v>
       </c>
       <c r="X28">
         <v>0.01670626856245372</v>
@@ -2716,7 +2716,7 @@
         <v>-0.0818496976144365</v>
       </c>
       <c r="F31">
-        <v>-0.02368333613681217</v>
+        <v>-0.02368333613681228</v>
       </c>
       <c r="G31">
         <v>-0.03785226595077662</v>
@@ -2775,7 +2775,7 @@
         <v>0.1103891299386426</v>
       </c>
       <c r="E32">
-        <v>0.08397877265727671</v>
+        <v>0.08397877265727693</v>
       </c>
       <c r="F32">
         <v>0.130727051846844</v>
@@ -2802,7 +2802,7 @@
         <v>0.03068768889705598</v>
       </c>
       <c r="N32">
-        <v>0.03703750605382194</v>
+        <v>0.03703750605382172</v>
       </c>
       <c r="O32">
         <v>0.01373313138881249</v>
@@ -2843,7 +2843,7 @@
         <v>0.0297973904238471</v>
       </c>
       <c r="G33">
-        <v>-0.01445595797322796</v>
+        <v>-0.01445595797322785</v>
       </c>
       <c r="H33">
         <v>0.04778458245330874</v>
@@ -2905,7 +2905,7 @@
         <v>-0.004630125206981917</v>
       </c>
       <c r="G34">
-        <v>0.0319239637309372</v>
+        <v>0.03192396373093698</v>
       </c>
       <c r="H34">
         <v>0.0656284091894288</v>
@@ -2970,7 +2970,7 @@
         <v>0.01588687002735378</v>
       </c>
       <c r="H35">
-        <v>-0.0448850404324983</v>
+        <v>-0.04488504043249841</v>
       </c>
       <c r="I35">
         <v>0.00423806965358664</v>
@@ -2982,7 +2982,7 @@
         <v>0.008088604165785718</v>
       </c>
       <c r="L35">
-        <v>0.01748168073176437</v>
+        <v>0.01748168073176415</v>
       </c>
       <c r="M35">
         <v>-0.01036938868955073</v>
@@ -3003,7 +3003,7 @@
         <v>0.01126229901495712</v>
       </c>
       <c r="T35">
-        <v>0.1362498201386433</v>
+        <v>0.1362498201386435</v>
       </c>
       <c r="V35">
         <v>-0.005282493534576327</v>
@@ -3091,7 +3091,7 @@
         <v>0.06547733592907212</v>
       </c>
       <c r="G37">
-        <v>-0.02925220586514865</v>
+        <v>-0.02925220586514876</v>
       </c>
       <c r="H37">
         <v>-0.00948264486246797</v>
@@ -3392,7 +3392,7 @@
         <v>-0.06909680541051555</v>
       </c>
       <c r="D42">
-        <v>-0.08947322687166437</v>
+        <v>-0.08947322687166426</v>
       </c>
       <c r="E42">
         <v>-0.07434439073690324</v>
@@ -3401,7 +3401,7 @@
         <v>-0.09806286212096593</v>
       </c>
       <c r="G42">
-        <v>-0.06892591815024562</v>
+        <v>-0.06892591815024574</v>
       </c>
       <c r="H42">
         <v>-0.05761297013845512</v>
@@ -3658,7 +3658,7 @@
         <v>0.01344066081904982</v>
       </c>
       <c r="J46">
-        <v>-0.1120097801631397</v>
+        <v>-0.1120097801631398</v>
       </c>
       <c r="K46">
         <v>-0.1727756554258818</v>
@@ -3723,10 +3723,10 @@
         <v>-0.01261392312711773</v>
       </c>
       <c r="K47">
-        <v>-0.00632786982283462</v>
+        <v>-0.006327869822834398</v>
       </c>
       <c r="L47">
-        <v>-0.02014645483019328</v>
+        <v>-0.02014645483019306</v>
       </c>
       <c r="M47">
         <v>0.01066811385126276</v>
@@ -3767,7 +3767,7 @@
         <v>-0.02216020835604116</v>
       </c>
       <c r="E48">
-        <v>-0.01261883844924461</v>
+        <v>-0.0126188384492445</v>
       </c>
       <c r="F48">
         <v>-0.02480619047304711</v>
@@ -3803,7 +3803,7 @@
         <v>0.04567527319983022</v>
       </c>
       <c r="R48">
-        <v>0.006716589086925184</v>
+        <v>0.006716589086924962</v>
       </c>
       <c r="S48">
         <v>-0.01951237417802765</v>
@@ -3968,7 +3968,7 @@
         <v>0.02022785089327317</v>
       </c>
       <c r="J51">
-        <v>-0.05646312490379313</v>
+        <v>-0.05646312490379335</v>
       </c>
       <c r="K51">
         <v>-0.07160947450668753</v>
@@ -4098,7 +4098,7 @@
         <v>0.06734039859926932</v>
       </c>
       <c r="L53">
-        <v>0.004779110664825614</v>
+        <v>0.004779110664825836</v>
       </c>
       <c r="M53">
         <v>0.03509823497437803</v>
@@ -4166,7 +4166,7 @@
         <v>-0.06841125582809437</v>
       </c>
       <c r="N54">
-        <v>-0.07880490364628678</v>
+        <v>-0.07880490364628689</v>
       </c>
       <c r="O54">
         <v>-0.1101473237164717</v>
@@ -4210,7 +4210,7 @@
         <v>-0.01047709319227419</v>
       </c>
       <c r="H55">
-        <v>0.003675919097970715</v>
+        <v>0.003675919097970937</v>
       </c>
       <c r="I55">
         <v>-0.07040646926290028</v>
@@ -4260,7 +4260,7 @@
         <v>0.02142838527947766</v>
       </c>
       <c r="D56">
-        <v>-0.07543176987603806</v>
+        <v>-0.07543176987603817</v>
       </c>
       <c r="E56">
         <v>-0.05158264851978922</v>
@@ -4494,7 +4494,7 @@
         <v>-0.07272612167512327</v>
       </c>
       <c r="V59">
-        <v>-0.02774958974954078</v>
+        <v>-0.02774958974954089</v>
       </c>
       <c r="X59">
         <v>-0.02572176473832877</v>
@@ -4570,7 +4570,7 @@
         <v>-0.06943666100384427</v>
       </c>
       <c r="D61">
-        <v>-0.03227945047750813</v>
+        <v>-0.03227945047750824</v>
       </c>
       <c r="E61">
         <v>-0.09501832080794526</v>
@@ -4739,7 +4739,7 @@
         <v>0.02463091823255836</v>
       </c>
       <c r="T63">
-        <v>0.05194894895088908</v>
+        <v>0.05194894895088931</v>
       </c>
       <c r="V63">
         <v>-1.488606467203724E-06</v>
@@ -4780,7 +4780,7 @@
         <v>-0.05452199536191238</v>
       </c>
       <c r="L64">
-        <v>-0.1200605527328314</v>
+        <v>-0.1200605527328316</v>
       </c>
       <c r="M64">
         <v>-0.04870700191814115</v>
@@ -4848,7 +4848,7 @@
         <v>-0.0410917481268982</v>
       </c>
       <c r="N65">
-        <v>0.004282887380890887</v>
+        <v>0.004282887380890665</v>
       </c>
       <c r="O65">
         <v>-0.03457037910998384</v>
@@ -4895,7 +4895,7 @@
         <v>0.0080544730213159</v>
       </c>
       <c r="I66">
-        <v>0.08892837739253223</v>
+        <v>0.08892837739253201</v>
       </c>
       <c r="J66">
         <v>-0.05244468806254554</v>
@@ -5810,7 +5810,7 @@
         <v>0.01422348441534682</v>
       </c>
       <c r="D81">
-        <v>0.04139516612438943</v>
+        <v>0.0413951661243892</v>
       </c>
       <c r="E81">
         <v>-0.04403506553686443</v>
@@ -6250,7 +6250,7 @@
         <v>-0.03738258264316052</v>
       </c>
       <c r="F88">
-        <v>-0.02751345754514445</v>
+        <v>-0.02751345754514434</v>
       </c>
       <c r="G88">
         <v>-0.05175952099683545</v>
@@ -6489,7 +6489,7 @@
         <v>37164</v>
       </c>
       <c r="C92">
-        <v>0.09214105510211512</v>
+        <v>0.0921410551021149</v>
       </c>
       <c r="D92">
         <v>0.1545771267390745</v>
@@ -6667,7 +6667,7 @@
         <v>-0.0232162149691757</v>
       </c>
       <c r="X94">
-        <v>0.01891881143021656</v>
+        <v>0.01891881143021634</v>
       </c>
     </row>
     <row r="95" spans="1:24">
@@ -6681,7 +6681,7 @@
         <v>0.02676926144825775</v>
       </c>
       <c r="E95">
-        <v>0.02979525657492088</v>
+        <v>0.0297952565749211</v>
       </c>
       <c r="F95">
         <v>0.07583548789820704</v>
@@ -6690,7 +6690,7 @@
         <v>0.0175313077289736</v>
       </c>
       <c r="H95">
-        <v>0.02380176876119222</v>
+        <v>0.02380176876119244</v>
       </c>
       <c r="I95">
         <v>-0.05063303959277932</v>
@@ -6965,7 +6965,7 @@
         <v>-0.06732881389775147</v>
       </c>
       <c r="R99">
-        <v>-0.05995741486375095</v>
+        <v>-0.05995741486375106</v>
       </c>
       <c r="S99">
         <v>-0.1027687097564542</v>
@@ -6994,7 +6994,7 @@
         <v>-0.0005068257066773718</v>
       </c>
       <c r="F100">
-        <v>0.03917577950278184</v>
+        <v>0.03917577950278162</v>
       </c>
       <c r="G100">
         <v>0.02336044760345191</v>
@@ -7095,7 +7095,7 @@
         <v>-0.01844447072193256</v>
       </c>
       <c r="T101">
-        <v>0.07358872111564119</v>
+        <v>0.07358872111564141</v>
       </c>
       <c r="V101">
         <v>-0.007879846213892261</v>
@@ -7644,7 +7644,7 @@
         <v>0.04336336333486002</v>
       </c>
       <c r="P110">
-        <v>-0.004085182340054394</v>
+        <v>-0.004085182340054283</v>
       </c>
       <c r="R110">
         <v>-0.03601975865215035</v>
@@ -7839,13 +7839,13 @@
         <v>-0.0008581160968261781</v>
       </c>
       <c r="T113">
-        <v>-0.04853558811059744</v>
+        <v>-0.04853558811059755</v>
       </c>
       <c r="V113">
         <v>-0.03719161962766893</v>
       </c>
       <c r="X113">
-        <v>-0.01298698990013891</v>
+        <v>-0.0129869899001388</v>
       </c>
     </row>
     <row r="114" spans="1:24">
@@ -7868,7 +7868,7 @@
         <v>0.08018893444140662</v>
       </c>
       <c r="H114">
-        <v>0.08397393754863192</v>
+        <v>0.08397393754863169</v>
       </c>
       <c r="I114">
         <v>0.03864576820575039</v>
@@ -8004,7 +8004,7 @@
         <v>-0.006858982023031146</v>
       </c>
       <c r="L116">
-        <v>0.01198995021331739</v>
+        <v>0.01198995021331717</v>
       </c>
       <c r="M116">
         <v>0.01476645001090038</v>
@@ -8205,7 +8205,7 @@
         <v>-0.02737962635886793</v>
       </c>
       <c r="R119">
-        <v>-0.03467367327297033</v>
+        <v>-0.03467367327297022</v>
       </c>
       <c r="S119">
         <v>-0.02372870800278104</v>
@@ -8276,7 +8276,7 @@
         <v>0.01293294587963389</v>
       </c>
       <c r="V120">
-        <v>0.001073488070241879</v>
+        <v>0.001073488070241657</v>
       </c>
       <c r="X120">
         <v>-0.01043873001391227</v>
@@ -8290,7 +8290,7 @@
         <v>-0.00342516437439444</v>
       </c>
       <c r="D121">
-        <v>0.04795346813547918</v>
+        <v>0.0479534681354794</v>
       </c>
       <c r="E121">
         <v>0.1015170753988321</v>
@@ -8411,7 +8411,7 @@
         <v>37381</v>
       </c>
       <c r="C123">
-        <v>-0.006967263194518569</v>
+        <v>-0.006967263194518902</v>
       </c>
       <c r="D123">
         <v>0.02276646708017882</v>
@@ -8819,7 +8819,7 @@
         <v>0.02434892490788187</v>
       </c>
       <c r="O129">
-        <v>-0.00322761517688186</v>
+        <v>-0.003227615176881637</v>
       </c>
       <c r="P129">
         <v>-0.006849735999245432</v>
@@ -8984,7 +8984,7 @@
         <v>0.02064431824579249</v>
       </c>
       <c r="H132">
-        <v>0.002874374347364483</v>
+        <v>0.002874374347364705</v>
       </c>
       <c r="I132">
         <v>0.006991769729835173</v>
@@ -9123,7 +9123,7 @@
         <v>-0.01170004634331567</v>
       </c>
       <c r="M134">
-        <v>-0.1712869187361608</v>
+        <v>-0.1712869187361609</v>
       </c>
       <c r="N134">
         <v>-0.1670806556930537</v>
@@ -9135,7 +9135,7 @@
         <v>-0.1130581167958545</v>
       </c>
       <c r="R134">
-        <v>-0.1002405550719579</v>
+        <v>-0.1002405550719578</v>
       </c>
       <c r="S134">
         <v>-0.08779564092522052</v>
@@ -9194,7 +9194,7 @@
         <v>0.1084333629760961</v>
       </c>
       <c r="P135">
-        <v>0.08302389712464286</v>
+        <v>0.08302389712464309</v>
       </c>
       <c r="R135">
         <v>-0.04953095411231589</v>
@@ -9324,7 +9324,7 @@
         <v>0.06708953938425566</v>
       </c>
       <c r="S137">
-        <v>0.06549615322428726</v>
+        <v>0.06549615322428748</v>
       </c>
       <c r="T137">
         <v>0.03806262946877714</v>
@@ -9498,7 +9498,7 @@
         <v>-0.009302145353393243</v>
       </c>
       <c r="N140">
-        <v>-0.04227078534179818</v>
+        <v>-0.04227078534179807</v>
       </c>
       <c r="O140">
         <v>-0.03881206186141994</v>
@@ -9811,7 +9811,7 @@
         <v>-0.00105087208484278</v>
       </c>
       <c r="O145">
-        <v>-0.04323353540991748</v>
+        <v>-0.04323353540991737</v>
       </c>
       <c r="P145">
         <v>0.007312298993102262</v>
@@ -9902,7 +9902,7 @@
         <v>-0.05155115404146304</v>
       </c>
       <c r="D147">
-        <v>0.107917563081293</v>
+        <v>0.1079175630812927</v>
       </c>
       <c r="E147">
         <v>0.1035472104273456</v>
@@ -9911,7 +9911,7 @@
         <v>0.1670036965093649</v>
       </c>
       <c r="G147">
-        <v>0.1506584757546821</v>
+        <v>0.1506584757546818</v>
       </c>
       <c r="H147">
         <v>0.08664458103623929</v>
@@ -9944,7 +9944,7 @@
         <v>0.0405669401506521</v>
       </c>
       <c r="S147">
-        <v>0.05795657977139124</v>
+        <v>0.05795657977139101</v>
       </c>
       <c r="T147">
         <v>-0.01171571644630354</v>
@@ -10068,7 +10068,7 @@
         <v>-0.05981220488973271</v>
       </c>
       <c r="S149">
-        <v>-0.01620194715887568</v>
+        <v>-0.01620194715887546</v>
       </c>
       <c r="T149">
         <v>0.06096044805621181</v>
@@ -10242,7 +10242,7 @@
         <v>-0.02660094455367168</v>
       </c>
       <c r="N152">
-        <v>-0.02057508981199085</v>
+        <v>-0.02057508981199097</v>
       </c>
       <c r="O152">
         <v>0.06609944934643885</v>
@@ -10505,7 +10505,7 @@
         <v>0.02215444746761275</v>
       </c>
       <c r="T156">
-        <v>-0.04394899786138307</v>
+        <v>-0.04394899786138318</v>
       </c>
       <c r="V156">
         <v>0.01028473205416702</v>
@@ -10953,7 +10953,7 @@
         <v>37668</v>
       </c>
       <c r="C164">
-        <v>0.006969033729308016</v>
+        <v>0.006969033729308238</v>
       </c>
       <c r="D164">
         <v>0.007411787791044899</v>
@@ -10989,7 +10989,7 @@
         <v>-0.02525657704030371</v>
       </c>
       <c r="O164">
-        <v>0.006534627592013287</v>
+        <v>0.006534627592013065</v>
       </c>
       <c r="P164">
         <v>0.002698264478597112</v>
@@ -11299,7 +11299,7 @@
         <v>0.103972550670717</v>
       </c>
       <c r="O169">
-        <v>0.1122059395915311</v>
+        <v>0.1122059395915316</v>
       </c>
       <c r="P169">
         <v>0.0468156824860575</v>
@@ -11402,7 +11402,7 @@
         <v>0.05110101719846627</v>
       </c>
       <c r="H171">
-        <v>-0.003800644095768413</v>
+        <v>-0.003800644095768302</v>
       </c>
       <c r="I171">
         <v>0.03087436638371566</v>
@@ -11417,7 +11417,7 @@
         <v>0.03038021831361304</v>
       </c>
       <c r="M171">
-        <v>0.008017334493156447</v>
+        <v>0.008017334493156225</v>
       </c>
       <c r="N171">
         <v>0.03112152481880659</v>
@@ -11511,7 +11511,7 @@
         <v>37731</v>
       </c>
       <c r="C173">
-        <v>0.01609849902712046</v>
+        <v>0.01609849902712068</v>
       </c>
       <c r="D173">
         <v>0.09077178963339994</v>
@@ -11535,7 +11535,7 @@
         <v>0.05081507181204503</v>
       </c>
       <c r="K173">
-        <v>0.08690325651856057</v>
+        <v>0.08690325651856035</v>
       </c>
       <c r="L173">
         <v>0.009065102095141109</v>
@@ -11762,7 +11762,7 @@
         <v>0.06071434063040981</v>
       </c>
       <c r="D177">
-        <v>0.05374844881145413</v>
+        <v>0.05374844881145435</v>
       </c>
       <c r="E177">
         <v>0.03889516622463862</v>
@@ -11898,7 +11898,7 @@
         <v>0.04937207147971101</v>
       </c>
       <c r="H179">
-        <v>-0.0350474452311349</v>
+        <v>-0.03504744523113457</v>
       </c>
       <c r="I179">
         <v>0.02114084926302162</v>
@@ -12309,7 +12309,7 @@
         <v>0.03052872878330914</v>
       </c>
       <c r="X185">
-        <v>0.01262147220148502</v>
+        <v>0.0126214722014848</v>
       </c>
     </row>
     <row r="186" spans="1:24">
@@ -12329,7 +12329,7 @@
         <v>0.003257109521354495</v>
       </c>
       <c r="G186">
-        <v>-0.008884178661690667</v>
+        <v>-0.008884178661690556</v>
       </c>
       <c r="H186">
         <v>-0.003550756045663905</v>
@@ -12663,7 +12663,7 @@
         <v>-0.05951543998061171</v>
       </c>
       <c r="O191">
-        <v>-0.005168770298114023</v>
+        <v>-0.005168770298113801</v>
       </c>
       <c r="P191">
         <v>-0.008144582173719161</v>
@@ -12899,7 +12899,7 @@
         <v>0.0330651964890627</v>
       </c>
       <c r="K195">
-        <v>0.07204246276076098</v>
+        <v>0.07204246276076121</v>
       </c>
       <c r="L195">
         <v>0.02190345897590573</v>
@@ -13014,7 +13014,7 @@
         <v>0.03858088671090698</v>
       </c>
       <c r="H197">
-        <v>0.02336232484276679</v>
+        <v>0.02336232484276657</v>
       </c>
       <c r="I197">
         <v>0.03560220932511382</v>
@@ -13171,7 +13171,7 @@
         <v>-0.01044209150244724</v>
       </c>
       <c r="T199">
-        <v>-0.03927229158776813</v>
+        <v>-0.03927229158776824</v>
       </c>
       <c r="V199">
         <v>0.006199262113437909</v>
@@ -13628,7 +13628,7 @@
         <v>0.003718624292477823</v>
       </c>
       <c r="F207">
-        <v>0.009852441172681692</v>
+        <v>0.009852441172681914</v>
       </c>
       <c r="G207">
         <v>0.02082485266011536</v>
@@ -13915,7 +13915,7 @@
         <v>-0.006477934301186372</v>
       </c>
       <c r="T211">
-        <v>0.08082769221172237</v>
+        <v>0.08082769221172215</v>
       </c>
       <c r="V211">
         <v>0.007651420154953792</v>
@@ -14018,7 +14018,7 @@
         <v>-0.01886468604022751</v>
       </c>
       <c r="L213">
-        <v>0.01531603817155514</v>
+        <v>0.01531603817155536</v>
       </c>
       <c r="M213">
         <v>0.05054677464598467</v>
@@ -14493,7 +14493,7 @@
         <v>-0.0198422842305146</v>
       </c>
       <c r="E221">
-        <v>-0.004575376948269816</v>
+        <v>-0.004575376948270038</v>
       </c>
       <c r="F221">
         <v>-0.005851965626319067</v>
@@ -14753,7 +14753,7 @@
         <v>-0.03021720236831893</v>
       </c>
       <c r="I225">
-        <v>-0.01424042178367591</v>
+        <v>-0.01424042178367602</v>
       </c>
       <c r="J225">
         <v>-0.02213809123335508</v>
@@ -14771,7 +14771,7 @@
         <v>0.05674108596548932</v>
       </c>
       <c r="O225">
-        <v>0.05489635124548964</v>
+        <v>0.05489635124548942</v>
       </c>
       <c r="P225">
         <v>0.03321626070044026</v>
@@ -14972,7 +14972,7 @@
         <v>0.03452206368109079</v>
       </c>
       <c r="V228">
-        <v>-0.01339465306683396</v>
+        <v>-0.01339465306683407</v>
       </c>
       <c r="X228">
         <v>-0.007765797582406808</v>
@@ -15695,7 +15695,7 @@
         <v>0.00298839527257555</v>
       </c>
       <c r="M240">
-        <v>-0.008433413211823226</v>
+        <v>-0.008433413211823004</v>
       </c>
       <c r="N240">
         <v>-0.01052521422215191</v>
@@ -15775,7 +15775,7 @@
         <v>-0.02501746931453774</v>
       </c>
       <c r="T241">
-        <v>-0.07915839280479797</v>
+        <v>-0.07915839280479808</v>
       </c>
       <c r="V241">
         <v>-0.04738397396362881</v>
@@ -15813,7 +15813,7 @@
         <v>-0.003547539023273982</v>
       </c>
       <c r="K242">
-        <v>0.01004155815094365</v>
+        <v>0.01004155815094343</v>
       </c>
       <c r="L242">
         <v>-0.001583168116223721</v>
@@ -15887,7 +15887,7 @@
         <v>0.01894091978412793</v>
       </c>
       <c r="O243">
-        <v>0.03341586433361576</v>
+        <v>0.03341586433361599</v>
       </c>
       <c r="P243">
         <v>0.007346389797016961</v>
@@ -15952,7 +15952,7 @@
         <v>0.02867012347086262</v>
       </c>
       <c r="O244">
-        <v>-0.02018234990126144</v>
+        <v>-0.02018234990126122</v>
       </c>
       <c r="P244">
         <v>0.00419910394087597</v>
@@ -16404,7 +16404,7 @@
         <v>0.02277697217470664</v>
       </c>
       <c r="N251">
-        <v>-0.04362464473856709</v>
+        <v>-0.04362464473856698</v>
       </c>
       <c r="O251">
         <v>0.005272881428022513</v>
@@ -17051,7 +17051,7 @@
         <v>0.0166251918033633</v>
       </c>
       <c r="M261">
-        <v>0.0003143016468547533</v>
+        <v>0.0003143016468545312</v>
       </c>
       <c r="N261">
         <v>0.01242678329866465</v>
@@ -18061,7 +18061,7 @@
         <v>38459</v>
       </c>
       <c r="C277">
-        <v>-0.02615582995170973</v>
+        <v>-0.02615582995170951</v>
       </c>
       <c r="D277">
         <v>-0.01444610681194947</v>
@@ -18082,7 +18082,7 @@
         <v>-0.007219569206878051</v>
       </c>
       <c r="J277">
-        <v>-0.05702680756715572</v>
+        <v>-0.05702680756715583</v>
       </c>
       <c r="K277">
         <v>-0.0703853896938198</v>
@@ -18277,7 +18277,7 @@
         <v>0.004883829716157972</v>
       </c>
       <c r="J280">
-        <v>-0.0197601117321955</v>
+        <v>-0.01976011173219527</v>
       </c>
       <c r="K280">
         <v>-0.04884046947343335</v>
@@ -19752,7 +19752,7 @@
         <v>-0.02322847311706022</v>
       </c>
       <c r="O302">
-        <v>-0.04998117369192046</v>
+        <v>-0.04998117369192057</v>
       </c>
       <c r="P302">
         <v>-0.06200744453462925</v>
@@ -20080,7 +20080,7 @@
         <v>-0.007331403575115081</v>
       </c>
       <c r="K307">
-        <v>0.05476058939892692</v>
+        <v>0.0547605893989267</v>
       </c>
       <c r="L307">
         <v>0.02032563148110134</v>
@@ -20284,7 +20284,7 @@
         <v>-0.02266544481962263</v>
       </c>
       <c r="K310">
-        <v>-0.00848154775268406</v>
+        <v>-0.008481547752683838</v>
       </c>
       <c r="L310">
         <v>0.003953370198535477</v>
@@ -20855,7 +20855,7 @@
         <v>0.01182737734345229</v>
       </c>
       <c r="T318">
-        <v>-0.05334586319314494</v>
+        <v>-0.05334586319314505</v>
       </c>
       <c r="U318">
         <v>0.08518838202685663</v>
@@ -21109,7 +21109,7 @@
         <v>-0.01659080760345166</v>
       </c>
       <c r="N322">
-        <v>0.02130216397940199</v>
+        <v>0.02130216397940221</v>
       </c>
       <c r="O322">
         <v>-0.02635267985705247</v>
@@ -21476,7 +21476,7 @@
         <v>0.007403718310525553</v>
       </c>
       <c r="X327">
-        <v>-0.006230379960487809</v>
+        <v>-0.00623037996048792</v>
       </c>
     </row>
     <row r="328" spans="1:24">
@@ -21762,7 +21762,7 @@
         <v>-0.002545184901630138</v>
       </c>
       <c r="E332">
-        <v>0.027985524556571</v>
+        <v>0.02798552455657077</v>
       </c>
       <c r="F332">
         <v>0.01101742183378684</v>
@@ -22274,7 +22274,7 @@
         <v>-0.01190510666280065</v>
       </c>
       <c r="Q339">
-        <v>0.002361277172066467</v>
+        <v>0.002361277172066689</v>
       </c>
       <c r="R339">
         <v>-1.334192993862615E-07</v>
@@ -22345,7 +22345,7 @@
         <v>0.05231750660117807</v>
       </c>
       <c r="R340">
-        <v>0.05706065215458289</v>
+        <v>0.05706065215458311</v>
       </c>
       <c r="S340">
         <v>0.03849090805370303</v>
@@ -22490,7 +22490,7 @@
         <v>-0.08537865328492489</v>
       </c>
       <c r="U342">
-        <v>-0.04031380583492938</v>
+        <v>-0.04031380583492961</v>
       </c>
       <c r="V342">
         <v>-0.04334594913189938</v>
@@ -22522,10 +22522,10 @@
         <v>0.001454450823933806</v>
       </c>
       <c r="I343">
-        <v>0.05046572095605106</v>
+        <v>0.05046572095605129</v>
       </c>
       <c r="J343">
-        <v>0.01634535665136716</v>
+        <v>0.01634535665136738</v>
       </c>
       <c r="K343">
         <v>0.02998860750027155</v>
@@ -22859,7 +22859,7 @@
         <v>0.0008227895042527411</v>
       </c>
       <c r="H348">
-        <v>0.03484156774479419</v>
+        <v>0.03484156774479441</v>
       </c>
       <c r="I348">
         <v>-0.006828823791239058</v>
@@ -23557,7 +23557,7 @@
         <v>-0.005281965825211898</v>
       </c>
       <c r="N358">
-        <v>-0.02461476463957424</v>
+        <v>-0.02461476463957413</v>
       </c>
       <c r="O358">
         <v>-0.02148014421981104</v>
@@ -23897,7 +23897,7 @@
         <v>-0.0003040714948525647</v>
       </c>
       <c r="N363">
-        <v>-0.09655517452768592</v>
+        <v>-0.09655517452768581</v>
       </c>
       <c r="O363">
         <v>-0.0167841656561778</v>
@@ -24264,7 +24264,7 @@
         <v>0.05296844742452511</v>
       </c>
       <c r="X368">
-        <v>0.01490983423463188</v>
+        <v>0.0149098342346321</v>
       </c>
     </row>
     <row r="369" spans="1:24">
@@ -24518,7 +24518,7 @@
         <v>2.492293105094134E-05</v>
       </c>
       <c r="Q372">
-        <v>-0.01246060687856609</v>
+        <v>-0.01246060687856587</v>
       </c>
       <c r="R372">
         <v>-0.009725554287128069</v>
@@ -24636,7 +24636,7 @@
         <v>-0.00193667448705015</v>
       </c>
       <c r="K374">
-        <v>-0.01687679292697364</v>
+        <v>-0.01687679292697353</v>
       </c>
       <c r="L374">
         <v>-0.008823370722193413</v>
@@ -24908,7 +24908,7 @@
         <v>0.06477427592863982</v>
       </c>
       <c r="K378">
-        <v>0.08990798648310672</v>
+        <v>0.08990798648310649</v>
       </c>
       <c r="L378">
         <v>0.05151938733729788</v>
@@ -25130,7 +25130,7 @@
         <v>0.002460232195845569</v>
       </c>
       <c r="Q381">
-        <v>0.03102622067808269</v>
+        <v>0.03102622067808292</v>
       </c>
       <c r="R381">
         <v>0.01851690755289059</v>
@@ -25316,7 +25316,7 @@
         <v>0.01364385277659319</v>
       </c>
       <c r="K384">
-        <v>0.01835119069941316</v>
+        <v>0.01835119069941293</v>
       </c>
       <c r="L384">
         <v>0.01464180799866122</v>
@@ -26771,7 +26771,7 @@
         <v>-0.02884819724076826</v>
       </c>
       <c r="T405">
-        <v>0.06465457614844983</v>
+        <v>0.06465457614845027</v>
       </c>
       <c r="U405">
         <v>0.01280086710616124</v>
@@ -26957,7 +26957,7 @@
         <v>-0.02593344630055516</v>
       </c>
       <c r="N408">
-        <v>-0.04710932290593239</v>
+        <v>-0.04710932290593228</v>
       </c>
       <c r="O408">
         <v>-0.007475200062141196</v>
@@ -27022,7 +27022,7 @@
         <v>0.02076637767178191</v>
       </c>
       <c r="M409">
-        <v>0.00108938015030402</v>
+        <v>0.001089380150304242</v>
       </c>
       <c r="N409">
         <v>0.009970009152527437</v>
@@ -27202,7 +27202,7 @@
         <v>0.01649362604345539</v>
       </c>
       <c r="E412">
-        <v>0.0184365318824482</v>
+        <v>0.01843653188244843</v>
       </c>
       <c r="F412">
         <v>0.008867586993049681</v>
@@ -27350,7 +27350,7 @@
         <v>0.05728524042486494</v>
       </c>
       <c r="I414">
-        <v>0.05155704180459564</v>
+        <v>0.05155704180459542</v>
       </c>
       <c r="J414">
         <v>0.04693251376229712</v>
@@ -27492,13 +27492,13 @@
         <v>-0.03313664005019556</v>
       </c>
       <c r="K416">
-        <v>-0.02689124673993293</v>
+        <v>-0.02689124673993315</v>
       </c>
       <c r="L416">
         <v>-0.02991249084274816</v>
       </c>
       <c r="M416">
-        <v>-0.001330856410931003</v>
+        <v>-0.001330856410930781</v>
       </c>
       <c r="N416">
         <v>-0.05327804952825321</v>
@@ -27664,7 +27664,7 @@
         <v>0.001662780316503687</v>
       </c>
       <c r="X418">
-        <v>-0.004021708005024771</v>
+        <v>-0.004021708005024549</v>
       </c>
     </row>
     <row r="419" spans="1:24">
@@ -27823,7 +27823,7 @@
         <v>-0.1439081147339597</v>
       </c>
       <c r="H421">
-        <v>-0.05512406982355844</v>
+        <v>-0.05512406982355855</v>
       </c>
       <c r="I421">
         <v>-0.09645362108286493</v>
@@ -27885,7 +27885,7 @@
         <v>0.102299431997027</v>
       </c>
       <c r="F422">
-        <v>0.09758044996361104</v>
+        <v>0.09758044996361126</v>
       </c>
       <c r="G422">
         <v>0.089569788637476</v>
@@ -27924,7 +27924,7 @@
         <v>-0.01965024529257497</v>
       </c>
       <c r="S422">
-        <v>-0.02691483958540741</v>
+        <v>-0.02691483958540763</v>
       </c>
       <c r="T422">
         <v>-0.1942859656194228</v>
@@ -27971,7 +27971,7 @@
         <v>-0.01309116641714303</v>
       </c>
       <c r="L423">
-        <v>0.01941913004321205</v>
+        <v>0.01941913004321227</v>
       </c>
       <c r="M423">
         <v>0.01440874889242605</v>
@@ -28237,7 +28237,7 @@
         <v>-0.07029217721500847</v>
       </c>
       <c r="J427">
-        <v>-0.04546739385022847</v>
+        <v>-0.04546739385022835</v>
       </c>
       <c r="K427">
         <v>-0.04684326690776996</v>
@@ -28320,7 +28320,7 @@
         <v>-0.04174090039892164</v>
       </c>
       <c r="O428">
-        <v>-0.04928212504297991</v>
+        <v>-0.04928212504298002</v>
       </c>
       <c r="P428">
         <v>-0.05194777964870434</v>
@@ -28506,7 +28506,7 @@
         <v>-0.01595020746830578</v>
       </c>
       <c r="I431">
-        <v>-0.09830989987452354</v>
+        <v>-0.09830989987452365</v>
       </c>
       <c r="J431">
         <v>-0.08450642709763734</v>
@@ -28539,7 +28539,7 @@
         <v>0.0005014424258713568</v>
       </c>
       <c r="T431">
-        <v>0.07308358358430112</v>
+        <v>0.07308358358430089</v>
       </c>
       <c r="U431">
         <v>0.01044899949863565</v>
@@ -28627,7 +28627,7 @@
         <v>-0.04185247746424658</v>
       </c>
       <c r="D433">
-        <v>-0.01746960607572789</v>
+        <v>-0.01746960607572801</v>
       </c>
       <c r="E433">
         <v>-0.06671002100843249</v>
@@ -28675,7 +28675,7 @@
         <v>0.02651533645638393</v>
       </c>
       <c r="T433">
-        <v>-0.03880417663129121</v>
+        <v>-0.03880417663129143</v>
       </c>
       <c r="U433">
         <v>-0.02895444686646009</v>
@@ -28908,7 +28908,7 @@
         <v>-0.07891457976084149</v>
       </c>
       <c r="G437">
-        <v>-0.1045854593083932</v>
+        <v>-0.1045854593083934</v>
       </c>
       <c r="H437">
         <v>-0.01913683129560662</v>
@@ -29050,7 +29050,7 @@
         <v>-0.003358036369332074</v>
       </c>
       <c r="I439">
-        <v>-0.04386924937050662</v>
+        <v>-0.04386924937050674</v>
       </c>
       <c r="J439">
         <v>-0.07748165436289267</v>
@@ -29210,13 +29210,13 @@
         <v>-0.0221937937419302</v>
       </c>
       <c r="Q441">
-        <v>-0.03158184681737486</v>
+        <v>-0.03158184681737497</v>
       </c>
       <c r="R441">
         <v>0.003530656890514017</v>
       </c>
       <c r="S441">
-        <v>-0.04992422727383405</v>
+        <v>-0.04992422727383417</v>
       </c>
       <c r="T441">
         <v>-0.01647742514088846</v>
@@ -29313,7 +29313,7 @@
         <v>-0.04345653066490107</v>
       </c>
       <c r="F443">
-        <v>-0.08999322958717215</v>
+        <v>-0.08999322958717204</v>
       </c>
       <c r="G443">
         <v>-0.05761677158727219</v>
@@ -29470,7 +29470,7 @@
         <v>-0.007707336240700524</v>
       </c>
       <c r="M445">
-        <v>0.02438327179086608</v>
+        <v>0.0243832717908663</v>
       </c>
       <c r="N445">
         <v>0.02719924634985937</v>
@@ -29511,7 +29511,7 @@
         <v>0.028095709653426</v>
       </c>
       <c r="D446">
-        <v>-0.06975150626137649</v>
+        <v>-0.06975150626137661</v>
       </c>
       <c r="E446">
         <v>-0.06088904020220964</v>
@@ -29621,7 +29621,7 @@
         <v>-0.06253307295041999</v>
       </c>
       <c r="R447">
-        <v>-0.06720766272001522</v>
+        <v>-0.0672076627200151</v>
       </c>
       <c r="S447">
         <v>-0.03300799308049462</v>
@@ -29754,7 +29754,7 @@
         <v>-0.02423559337857595</v>
       </c>
       <c r="Q449">
-        <v>-0.03282831050993507</v>
+        <v>-0.03282831050993495</v>
       </c>
       <c r="R449">
         <v>0.02119726772647645</v>
@@ -29976,7 +29976,7 @@
         <v>0.005109414296424752</v>
       </c>
       <c r="X452">
-        <v>-0.004622043529814657</v>
+        <v>-0.004622043529814768</v>
       </c>
     </row>
     <row r="453" spans="1:24">
@@ -30159,7 +30159,7 @@
         <v>-0.01399487341196359</v>
       </c>
       <c r="P455">
-        <v>0.02486143868212931</v>
+        <v>0.02486143868212909</v>
       </c>
       <c r="Q455">
         <v>0.00815087494527611</v>
@@ -30200,7 +30200,7 @@
         <v>0.110848421802904</v>
       </c>
       <c r="G456">
-        <v>0.1497778302223398</v>
+        <v>0.1497778302223396</v>
       </c>
       <c r="H456">
         <v>0.04713699841496566</v>
@@ -30245,7 +30245,7 @@
         <v>0.02625194751268101</v>
       </c>
       <c r="V456">
-        <v>-0.08906609275643063</v>
+        <v>-0.08906609275643051</v>
       </c>
       <c r="X456">
         <v>0.002700804322151917</v>
@@ -30277,7 +30277,7 @@
         <v>-0.06256205990941233</v>
       </c>
       <c r="J457">
-        <v>0.06309704418154749</v>
+        <v>0.06309704418154727</v>
       </c>
       <c r="K457">
         <v>-0.09040762936960978</v>
@@ -30336,7 +30336,7 @@
         <v>-0.06048977293569491</v>
       </c>
       <c r="G458">
-        <v>-0.08932984100354335</v>
+        <v>-0.08932984100354358</v>
       </c>
       <c r="H458">
         <v>-0.07166077958060824</v>
@@ -30378,7 +30378,7 @@
         <v>-0.2430601392564811</v>
       </c>
       <c r="U458">
-        <v>-0.1023791853369295</v>
+        <v>-0.1023791853369294</v>
       </c>
       <c r="V458">
         <v>-0.03941564632405392</v>
@@ -30502,7 +30502,7 @@
         <v>0.09108425651743501</v>
       </c>
       <c r="Q460">
-        <v>0.08657649611148788</v>
+        <v>0.08657649611148766</v>
       </c>
       <c r="R460">
         <v>0.07815896492697938</v>
@@ -30567,7 +30567,7 @@
         <v>-0.04035180890474421</v>
       </c>
       <c r="P461">
-        <v>0.01469711975264509</v>
+        <v>0.01469711975264487</v>
       </c>
       <c r="Q461">
         <v>-0.03685377297593606</v>
@@ -30585,7 +30585,7 @@
         <v>-0.08925223357232781</v>
       </c>
       <c r="V461">
-        <v>-0.08232314399062435</v>
+        <v>-0.08232314399062446</v>
       </c>
       <c r="X461">
         <v>-0.06781191763568495</v>
@@ -30611,7 +30611,7 @@
         <v>0.1381039393711372</v>
       </c>
       <c r="H462">
-        <v>0.06371963942146341</v>
+        <v>0.06371963942146364</v>
       </c>
       <c r="I462">
         <v>0.1015849980131227</v>
@@ -30712,7 +30712,7 @@
         <v>-0.01528112957252603</v>
       </c>
       <c r="S463">
-        <v>-0.004224650154497689</v>
+        <v>-0.004224650154497467</v>
       </c>
       <c r="T463">
         <v>-0.08690319939831914</v>
@@ -30774,7 +30774,7 @@
         <v>-0.003649876985943434</v>
       </c>
       <c r="Q464">
-        <v>-0.07566741060535975</v>
+        <v>-0.07566741060535986</v>
       </c>
       <c r="R464">
         <v>-0.001770387613633795</v>
@@ -30824,7 +30824,7 @@
         <v>-0.201109319716092</v>
       </c>
       <c r="K465">
-        <v>-0.1645890170939395</v>
+        <v>-0.1645890170939394</v>
       </c>
       <c r="L465">
         <v>-0.09228019124832454</v>
@@ -30936,7 +30936,7 @@
         <v>39789</v>
       </c>
       <c r="C467">
-        <v>-0.005495013589771891</v>
+        <v>-0.005495013589772002</v>
       </c>
       <c r="D467">
         <v>0.07153405417727177</v>
@@ -31344,7 +31344,7 @@
         <v>39831</v>
       </c>
       <c r="C473">
-        <v>-0.1951296867325901</v>
+        <v>-0.1951296867325902</v>
       </c>
       <c r="D473">
         <v>-0.1803132734032812</v>
@@ -31421,7 +31421,7 @@
         <v>0.06397892825219431</v>
       </c>
       <c r="F474">
-        <v>-0.130919785368936</v>
+        <v>-0.1309197853689362</v>
       </c>
       <c r="G474">
         <v>-0.008571832881544506</v>
@@ -31439,7 +31439,7 @@
         <v>0.2001289427420951</v>
       </c>
       <c r="L474">
-        <v>-0.1076338243971731</v>
+        <v>-0.107633824397173</v>
       </c>
       <c r="M474">
         <v>-0.02559253926846128</v>
@@ -31602,7 +31602,7 @@
         <v>0.1064006334344778</v>
       </c>
       <c r="U476">
-        <v>0.09674262874855155</v>
+        <v>0.09674262874855133</v>
       </c>
       <c r="V476">
         <v>0.1497078949146053</v>
@@ -31767,7 +31767,7 @@
         <v>-0.2307696456374332</v>
       </c>
       <c r="H479">
-        <v>0.1210175579653909</v>
+        <v>0.1210175579653912</v>
       </c>
       <c r="I479">
         <v>0.1090749216952818</v>
@@ -31806,13 +31806,13 @@
         <v>-0.02072384168576535</v>
       </c>
       <c r="U479">
-        <v>-0.02441907572384117</v>
+        <v>-0.02441907572384105</v>
       </c>
       <c r="V479">
         <v>-0.1027780265209725</v>
       </c>
       <c r="X479">
-        <v>-0.04539980148583844</v>
+        <v>-0.04539980148583855</v>
       </c>
     </row>
     <row r="480" spans="1:24">
@@ -31841,7 +31841,7 @@
         <v>-0.2884295186257376</v>
       </c>
       <c r="J480">
-        <v>-0.1694118258537344</v>
+        <v>-0.1694118258537343</v>
       </c>
       <c r="K480">
         <v>-0.1207786355383244</v>
@@ -31965,7 +31965,7 @@
         <v>-0.02526214075280753</v>
       </c>
       <c r="F482">
-        <v>0.07465245154604183</v>
+        <v>0.07465245154604161</v>
       </c>
       <c r="G482">
         <v>0.4719103405693494</v>
@@ -32039,7 +32039,7 @@
         <v>-1.139475040656812E-06</v>
       </c>
       <c r="H483">
-        <v>0.05005226241823602</v>
+        <v>0.05005226241823579</v>
       </c>
       <c r="I483">
         <v>0.1143669418005546</v>
@@ -32048,7 +32048,7 @@
         <v>0.1105637418313381</v>
       </c>
       <c r="K483">
-        <v>0.2030634320073987</v>
+        <v>0.203063432007399</v>
       </c>
       <c r="L483">
         <v>0.08158587988777177</v>
@@ -32116,7 +32116,7 @@
         <v>0.1047363152471654</v>
       </c>
       <c r="K484">
-        <v>-0.01190844046546002</v>
+        <v>-0.01190844046546025</v>
       </c>
       <c r="L484">
         <v>0.1494531024541086</v>
@@ -32187,7 +32187,7 @@
         <v>0.05361626317220791</v>
       </c>
       <c r="L485">
-        <v>0.07390450978810126</v>
+        <v>0.07390450978810148</v>
       </c>
       <c r="M485">
         <v>-0.01418954263180106</v>
@@ -32208,7 +32208,7 @@
         <v>-0.01773484183866192</v>
       </c>
       <c r="S485">
-        <v>-0.03193686323525902</v>
+        <v>-0.03193686323525913</v>
       </c>
       <c r="T485">
         <v>0.03086480281840287</v>
@@ -32376,7 +32376,7 @@
         <v>-0.04395564687161513</v>
       </c>
       <c r="G488">
-        <v>-0.0689654430241029</v>
+        <v>-0.06896544302410279</v>
       </c>
       <c r="H488">
         <v>0.01781559293276525</v>
@@ -32772,7 +32772,7 @@
         <v>39978</v>
       </c>
       <c r="C494">
-        <v>-0.01618191322868445</v>
+        <v>-0.01618191322868467</v>
       </c>
       <c r="D494">
         <v>0.03222334961027951</v>
@@ -32805,7 +32805,7 @@
         <v>0.002323758558772315</v>
       </c>
       <c r="N494">
-        <v>0.01722840724229346</v>
+        <v>0.01722840724229324</v>
       </c>
       <c r="O494">
         <v>0.0003843107411414248</v>
@@ -33562,7 +33562,7 @@
         <v>0.002859895608336771</v>
       </c>
       <c r="Q505">
-        <v>0.01344715035796429</v>
+        <v>0.01344715035796407</v>
       </c>
       <c r="R505">
         <v>0.01362342247924131</v>
@@ -33624,7 +33624,7 @@
         <v>-0.02498532615324067</v>
       </c>
       <c r="O506">
-        <v>-0.03840826250546281</v>
+        <v>-0.0384082625054627</v>
       </c>
       <c r="P506">
         <v>-0.01340494950411564</v>
@@ -33656,7 +33656,7 @@
         <v>40069</v>
       </c>
       <c r="C507">
-        <v>0.04374679165036088</v>
+        <v>0.04374679165036111</v>
       </c>
       <c r="D507">
         <v>0.01911460846576096</v>
@@ -34088,7 +34088,7 @@
         <v>-0.02174955728248662</v>
       </c>
       <c r="K513">
-        <v>0.06092818998505756</v>
+        <v>0.06092818998505778</v>
       </c>
       <c r="L513">
         <v>0.001926104716215349</v>
@@ -34132,7 +34132,7 @@
         <v>40118</v>
       </c>
       <c r="C514">
-        <v>-0.06620909785385976</v>
+        <v>-0.06620909785385998</v>
       </c>
       <c r="D514">
         <v>-0.06933868681443023</v>
@@ -34236,10 +34236,10 @@
         <v>0.005300785191543866</v>
       </c>
       <c r="O515">
-        <v>0.05366911507466243</v>
+        <v>0.05366911507466265</v>
       </c>
       <c r="P515">
-        <v>0.0126958342720731</v>
+        <v>0.01269583427207288</v>
       </c>
       <c r="Q515">
         <v>0.02985383004987918</v>
@@ -34552,7 +34552,7 @@
         <v>-0.03992744328208386</v>
       </c>
       <c r="G520">
-        <v>-0.041262590957582</v>
+        <v>-0.04126259095758211</v>
       </c>
       <c r="H520">
         <v>-0.01660374060298431</v>
@@ -34845,7 +34845,7 @@
         <v>-0.00310507843145047</v>
       </c>
       <c r="N524">
-        <v>0.02693917916694777</v>
+        <v>0.02693917916694799</v>
       </c>
       <c r="O524">
         <v>0.03174615229045141</v>
@@ -34981,7 +34981,7 @@
         <v>-0.02106498696085013</v>
       </c>
       <c r="N526">
-        <v>-0.02719335109520682</v>
+        <v>-0.02719335109520671</v>
       </c>
       <c r="O526">
         <v>-0.01520162737524944</v>
@@ -35454,7 +35454,7 @@
         <v>-0.03281685509165233</v>
       </c>
       <c r="M533">
-        <v>0.002184838968383174</v>
+        <v>0.002184838968382952</v>
       </c>
       <c r="N533">
         <v>-0.02288324788269913</v>
@@ -35587,7 +35587,7 @@
         <v>-0.02632347933791046</v>
       </c>
       <c r="L535">
-        <v>-0.001758715034714808</v>
+        <v>-0.001758715034714919</v>
       </c>
       <c r="M535">
         <v>-0.01121266672367449</v>
@@ -35732,7 +35732,7 @@
         <v>0.009953154032255052</v>
       </c>
       <c r="O537">
-        <v>-0.01962336028803224</v>
+        <v>-0.01962336028803235</v>
       </c>
       <c r="P537">
         <v>0.01701035563328279</v>
@@ -35986,7 +35986,7 @@
         <v>-0.0674162067171663</v>
       </c>
       <c r="I541">
-        <v>-0.06773760094433412</v>
+        <v>-0.06773760094433423</v>
       </c>
       <c r="J541">
         <v>-0.01521973037335733</v>
@@ -36016,7 +36016,7 @@
         <v>-0.05329088948293503</v>
       </c>
       <c r="S541">
-        <v>-0.0437541236280492</v>
+        <v>-0.04375412362804909</v>
       </c>
       <c r="T541">
         <v>-0.09663415095122074</v>
@@ -36057,7 +36057,7 @@
         <v>0.03958425678239408</v>
       </c>
       <c r="J542">
-        <v>0.001679229941506044</v>
+        <v>0.001679229941505822</v>
       </c>
       <c r="K542">
         <v>-0.02414432687854517</v>
@@ -36175,7 +36175,7 @@
         <v>-0.0001592741175209245</v>
       </c>
       <c r="D544">
-        <v>-0.0008351406094960767</v>
+        <v>-0.0008351406094962988</v>
       </c>
       <c r="E544">
         <v>-0.01173499118025856</v>
@@ -36320,7 +36320,7 @@
         <v>0.01628691279893868</v>
       </c>
       <c r="G546">
-        <v>0.02374719221114518</v>
+        <v>0.02374719221114496</v>
       </c>
       <c r="H546">
         <v>0.01684536246136159</v>
@@ -36356,7 +36356,7 @@
         <v>0.03900094775906582</v>
       </c>
       <c r="S546">
-        <v>-0.08584347943659543</v>
+        <v>-0.08584347943659554</v>
       </c>
       <c r="T546">
         <v>-0.009590965290880771</v>
@@ -36572,7 +36572,7 @@
         <v>-0.05146188594782575</v>
       </c>
       <c r="X549">
-        <v>-0.05031689854726196</v>
+        <v>-0.05031689854726207</v>
       </c>
     </row>
     <row r="550" spans="1:24">
@@ -37677,7 +37677,7 @@
         <v>-0.001856556026495815</v>
       </c>
       <c r="F566">
-        <v>0.0007861843534411328</v>
+        <v>0.0007861843534409108</v>
       </c>
       <c r="G566">
         <v>0.01459887766543289</v>
@@ -37893,7 +37893,7 @@
         <v>-0.001814937374528647</v>
       </c>
       <c r="J569">
-        <v>0.005065521349629343</v>
+        <v>0.005065521349629565</v>
       </c>
       <c r="K569">
         <v>0.001955112715727569</v>
@@ -37973,7 +37973,7 @@
         <v>-0.01347390560844719</v>
       </c>
       <c r="N570">
-        <v>-0.01354340637018447</v>
+        <v>-0.01354340637018459</v>
       </c>
       <c r="O570">
         <v>-0.01330299925864975</v>
@@ -38062,7 +38062,7 @@
         <v>0.005319507987772587</v>
       </c>
       <c r="U571">
-        <v>-0.02881219858624706</v>
+        <v>-0.02881219858624717</v>
       </c>
       <c r="V571">
         <v>0.0662990664606784</v>
@@ -38109,7 +38109,7 @@
         <v>0.000381254402475939</v>
       </c>
       <c r="M572">
-        <v>-0.01038985572901618</v>
+        <v>-0.01038985572901607</v>
       </c>
       <c r="N572">
         <v>0.01794321503317153</v>
@@ -38218,7 +38218,7 @@
         <v>40538</v>
       </c>
       <c r="B574">
-        <v>0.03706309110286687</v>
+        <v>0.0370630911028671</v>
       </c>
       <c r="C574">
         <v>0.02752070370904236</v>
@@ -38393,7 +38393,7 @@
         <v>0.03644061037785207</v>
       </c>
       <c r="M576">
-        <v>0.01212652563945005</v>
+        <v>0.01212652563944983</v>
       </c>
       <c r="N576">
         <v>0.0474011760599673</v>
@@ -39428,7 +39428,7 @@
         <v>0.03200051609182641</v>
       </c>
       <c r="C591">
-        <v>-0.00452284598739594</v>
+        <v>-0.004522845987396051</v>
       </c>
       <c r="D591">
         <v>-0.03008073193169225</v>
@@ -39851,7 +39851,7 @@
         <v>40699</v>
       </c>
       <c r="B597">
-        <v>-0.04971133816552609</v>
+        <v>-0.04971133816552598</v>
       </c>
       <c r="C597">
         <v>-0.05116775679124641</v>
@@ -39964,7 +39964,7 @@
         <v>-0.01032890300708078</v>
       </c>
       <c r="P598">
-        <v>-0.01724540569966071</v>
+        <v>-0.01724540569966093</v>
       </c>
       <c r="Q598">
         <v>-0.01517407706855844</v>
@@ -40135,7 +40135,7 @@
         <v>40727</v>
       </c>
       <c r="B601">
-        <v>-0.05946570511677862</v>
+        <v>-0.05946570511677873</v>
       </c>
       <c r="C601">
         <v>0.07560497375732766</v>
@@ -40378,7 +40378,7 @@
         <v>0.1332389258589515</v>
       </c>
       <c r="L604">
-        <v>0.03035259036469085</v>
+        <v>0.03035259036469107</v>
       </c>
       <c r="M604">
         <v>-0.01082263563858821</v>
@@ -40508,7 +40508,7 @@
         <v>-0.127804179112273</v>
       </c>
       <c r="H606">
-        <v>-0.04969319403875105</v>
+        <v>-0.04969319403875117</v>
       </c>
       <c r="I606">
         <v>-0.09374409016146867</v>
@@ -40659,7 +40659,7 @@
         <v>-0.0404400738263524</v>
       </c>
       <c r="K608">
-        <v>-0.05269403346787693</v>
+        <v>-0.05269403346787715</v>
       </c>
       <c r="L608">
         <v>-0.05257102038831718</v>
@@ -40795,7 +40795,7 @@
         <v>-0.004810990757911693</v>
       </c>
       <c r="I610">
-        <v>-0.01585918717901802</v>
+        <v>-0.0158591871790178</v>
       </c>
       <c r="J610">
         <v>-0.03905770317773405</v>
@@ -41061,7 +41061,7 @@
         <v>-0.01988986721202013</v>
       </c>
       <c r="C614">
-        <v>0.0190304289329879</v>
+        <v>0.01903042893298768</v>
       </c>
       <c r="D614">
         <v>0.01964782657703901</v>
@@ -41206,7 +41206,7 @@
         <v>0.07141379466002773</v>
       </c>
       <c r="D616">
-        <v>0.05872265708002344</v>
+        <v>0.05872265708002322</v>
       </c>
       <c r="E616">
         <v>0.03876170843565174</v>
@@ -41467,7 +41467,7 @@
         <v>-0.02694010474106456</v>
       </c>
       <c r="T619">
-        <v>-0.01163131558827712</v>
+        <v>-0.01163131558827724</v>
       </c>
       <c r="U619">
         <v>-0.006664278406705915</v>
@@ -41591,7 +41591,7 @@
         <v>-0.02145691805322503</v>
       </c>
       <c r="N621">
-        <v>-0.02301160848724859</v>
+        <v>-0.0230116084872487</v>
       </c>
       <c r="O621">
         <v>-0.02835738663643428</v>
@@ -41703,10 +41703,10 @@
         <v>0.09985609664806083</v>
       </c>
       <c r="D623">
-        <v>0.07032747162312125</v>
+        <v>0.07032747162312147</v>
       </c>
       <c r="E623">
-        <v>0.1351820374529633</v>
+        <v>0.1351820374529635</v>
       </c>
       <c r="F623">
         <v>0.0929142031670851</v>
@@ -41952,7 +41952,7 @@
         <v>0.04551780798552674</v>
       </c>
       <c r="P626">
-        <v>0.0631236721262276</v>
+        <v>0.06312367212622783</v>
       </c>
       <c r="Q626">
         <v>0.03277282041672791</v>
@@ -42508,7 +42508,7 @@
         <v>-0.02543191708100223</v>
       </c>
       <c r="L634">
-        <v>0.04255862990504955</v>
+        <v>0.04255862990504933</v>
       </c>
       <c r="M634">
         <v>0.006036326745253451</v>
@@ -42665,7 +42665,7 @@
         <v>-0.01156295506022065</v>
       </c>
       <c r="Q636">
-        <v>-0.01074215748024643</v>
+        <v>-0.01074215748024665</v>
       </c>
       <c r="R636">
         <v>0.004858994252994187</v>
@@ -43008,7 +43008,7 @@
         <v>-0.01239076676641748</v>
       </c>
       <c r="M641">
-        <v>-0.00940025686000534</v>
+        <v>-0.009400256860005451</v>
       </c>
       <c r="N641">
         <v>-0.01346866026097127</v>
@@ -43422,7 +43422,7 @@
         <v>-0.06066831520707394</v>
       </c>
       <c r="I647">
-        <v>-0.07114957289515755</v>
+        <v>-0.07114957289515744</v>
       </c>
       <c r="J647">
         <v>-0.06501538664477535</v>
@@ -43626,7 +43626,7 @@
         <v>0.05480739084369102</v>
       </c>
       <c r="F650">
-        <v>0.07692209724792742</v>
+        <v>0.0769220972479272</v>
       </c>
       <c r="G650">
         <v>0.09373724229686808</v>
@@ -43736,7 +43736,7 @@
         <v>0.03460979341161874</v>
       </c>
       <c r="S651">
-        <v>0.05538067726728091</v>
+        <v>0.05538067726728069</v>
       </c>
       <c r="T651">
         <v>-0.01066739163245589</v>
@@ -43910,7 +43910,7 @@
         <v>-0.04328475070386895</v>
       </c>
       <c r="F654">
-        <v>-0.06356947417617453</v>
+        <v>-0.06356947417617465</v>
       </c>
       <c r="G654">
         <v>-0.03830796219946453</v>
@@ -44171,7 +44171,7 @@
         <v>0.03951975722020507</v>
       </c>
       <c r="V657">
-        <v>-0.01195461029741485</v>
+        <v>-0.01195461029741496</v>
       </c>
       <c r="X657">
         <v>0.01710650771572109</v>
@@ -44540,7 +44540,7 @@
         <v>0.01713101331999867</v>
       </c>
       <c r="C663">
-        <v>0.02638381590442074</v>
+        <v>0.02638381590442052</v>
       </c>
       <c r="D663">
         <v>0.0170606235716857</v>
@@ -44647,7 +44647,7 @@
         <v>-0.01815193344595623</v>
       </c>
       <c r="O664">
-        <v>-0.0004487018835742651</v>
+        <v>-0.0004487018835741541</v>
       </c>
       <c r="P664">
         <v>0.02646864506022939</v>
@@ -45321,7 +45321,7 @@
         <v>0.03636299086712569</v>
       </c>
       <c r="C674">
-        <v>0.02594889452927207</v>
+        <v>0.02594889452927185</v>
       </c>
       <c r="D674">
         <v>0.03264648270156023</v>
@@ -46046,7 +46046,7 @@
         <v>0.002800429979913588</v>
       </c>
       <c r="H684">
-        <v>0.01669373118180917</v>
+        <v>0.01669373118180895</v>
       </c>
       <c r="I684">
         <v>0.006861798408928976</v>
@@ -46511,7 +46511,7 @@
         <v>0.02765527816627178</v>
       </c>
       <c r="U690">
-        <v>-0.02070635933914378</v>
+        <v>-0.02070635933914355</v>
       </c>
       <c r="V690">
         <v>0.001249700036207502</v>
@@ -46552,7 +46552,7 @@
         <v>-0.05321515607726324</v>
       </c>
       <c r="K691">
-        <v>-0.05977073528566157</v>
+        <v>-0.05977073528566135</v>
       </c>
       <c r="L691">
         <v>-0.003428194946802243</v>
@@ -46670,7 +46670,7 @@
         <v>-0.0292592762755649</v>
       </c>
       <c r="C693">
-        <v>-0.01894813875590751</v>
+        <v>-0.01894813875590728</v>
       </c>
       <c r="D693">
         <v>-0.01679948951867927</v>
@@ -46812,7 +46812,7 @@
         <v>-0.07774997725062116</v>
       </c>
       <c r="C695">
-        <v>-0.008812263174063695</v>
+        <v>-0.008812263174063806</v>
       </c>
       <c r="D695">
         <v>-0.04606768094048475</v>
@@ -46993,7 +46993,7 @@
         <v>-0.04595774398048069</v>
       </c>
       <c r="P697">
-        <v>0.02295401023304722</v>
+        <v>0.022954010233047</v>
       </c>
       <c r="Q697">
         <v>0.03429151196719804</v>
@@ -47108,7 +47108,7 @@
         <v>0.0314908709757058</v>
       </c>
       <c r="G699">
-        <v>0.05538519332544567</v>
+        <v>0.05538519332544589</v>
       </c>
       <c r="H699">
         <v>-0.008692149641688296</v>
@@ -47173,7 +47173,7 @@
         <v>0.02134493570834262</v>
       </c>
       <c r="E700">
-        <v>0.02600461996934733</v>
+        <v>0.02600461996934711</v>
       </c>
       <c r="F700">
         <v>-0.014147142855927</v>
@@ -47286,7 +47286,7 @@
         <v>-0.02152192826944277</v>
       </c>
       <c r="S701">
-        <v>-0.01401650274517852</v>
+        <v>-0.01401650274517841</v>
       </c>
       <c r="T701">
         <v>0.01029897459142037</v>
@@ -47392,7 +47392,7 @@
         <v>-0.02316923799108028</v>
       </c>
       <c r="G703">
-        <v>-0.04612388979039395</v>
+        <v>-0.04612388979039406</v>
       </c>
       <c r="H703">
         <v>0.002210711314496017</v>
@@ -47419,7 +47419,7 @@
         <v>0.003952339237433655</v>
       </c>
       <c r="P703">
-        <v>-0.009512232283934052</v>
+        <v>-0.009512232283934163</v>
       </c>
       <c r="Q703">
         <v>0.003681660109217333</v>
@@ -47478,7 +47478,7 @@
         <v>-0.03561796943365936</v>
       </c>
       <c r="L704">
-        <v>-0.03620447090084289</v>
+        <v>-0.03620447090084278</v>
       </c>
       <c r="M704">
         <v>-0.02013908665513886</v>
@@ -47738,7 +47738,7 @@
         <v>0.03043536975382866</v>
       </c>
       <c r="D708">
-        <v>-0.0106223902038064</v>
+        <v>-0.01062239020380651</v>
       </c>
       <c r="E708">
         <v>0.02164800160027669</v>
@@ -49179,7 +49179,7 @@
         <v>-0.01024075743368247</v>
       </c>
       <c r="K728">
-        <v>-0.02683788763584516</v>
+        <v>-0.02683788763584527</v>
       </c>
       <c r="L728">
         <v>-0.03333365017077072</v>
@@ -49348,7 +49348,7 @@
         <v>0.02560720564123442</v>
       </c>
       <c r="T730">
-        <v>-0.009758580943381667</v>
+        <v>-0.009758580943381556</v>
       </c>
       <c r="U730">
         <v>0.03754698131478262</v>
@@ -50419,7 +50419,7 @@
         <v>-0.02797890038695938</v>
       </c>
       <c r="V745">
-        <v>-0.01066933616515053</v>
+        <v>-0.01066933616515076</v>
       </c>
       <c r="X745">
         <v>0.004021227633931312</v>
@@ -50451,7 +50451,7 @@
         <v>-0.001205057349290883</v>
       </c>
       <c r="I746">
-        <v>-0.02986360718849657</v>
+        <v>-0.02986360718849645</v>
       </c>
       <c r="J746">
         <v>-0.06444511342416215</v>
@@ -50581,7 +50581,7 @@
         <v>-0.0007442318379627944</v>
       </c>
       <c r="E748">
-        <v>0.008692541773400508</v>
+        <v>0.008692541773400286</v>
       </c>
       <c r="F748">
         <v>-0.01238436801550025</v>
@@ -51211,7 +51211,7 @@
         <v>41819</v>
       </c>
       <c r="B757">
-        <v>-0.00710291239813754</v>
+        <v>-0.007102912398137318</v>
       </c>
       <c r="C757">
         <v>-0.001230727454205383</v>
@@ -51664,7 +51664,7 @@
         <v>0.01180602699876698</v>
       </c>
       <c r="K763">
-        <v>0.01107638235281883</v>
+        <v>0.01107638235281905</v>
       </c>
       <c r="L763">
         <v>0.002080743702933319</v>
@@ -52025,7 +52025,7 @@
         <v>-0.01185019350792138</v>
       </c>
       <c r="M768">
-        <v>0.0015319273299359</v>
+        <v>0.001531927329935678</v>
       </c>
       <c r="N768">
         <v>-0.007420168666015248</v>
@@ -52194,7 +52194,7 @@
         <v>-0.02890571745363346</v>
       </c>
       <c r="V770">
-        <v>-0.02335950232732242</v>
+        <v>-0.02335950232732231</v>
       </c>
       <c r="W770">
         <v>-0.03653207586086826</v>
@@ -52259,7 +52259,7 @@
         <v>-0.03095453402855464</v>
       </c>
       <c r="S771">
-        <v>-0.03742117184584459</v>
+        <v>-0.0374211718458447</v>
       </c>
       <c r="T771">
         <v>-0.01121509882908023</v>
@@ -52291,7 +52291,7 @@
         <v>-0.03839755400013967</v>
       </c>
       <c r="E772">
-        <v>-0.02951902312736243</v>
+        <v>-0.02951902312736254</v>
       </c>
       <c r="F772">
         <v>-0.04684830656435446</v>
@@ -52454,7 +52454,7 @@
         <v>0.05155198214184042</v>
       </c>
       <c r="J774">
-        <v>0.03640362315356493</v>
+        <v>0.03640362315356471</v>
       </c>
       <c r="K774">
         <v>0.0331124930482376</v>
@@ -52789,7 +52789,7 @@
         <v>-0.02611532595900534</v>
       </c>
       <c r="W778">
-        <v>-0.03796775623713577</v>
+        <v>-0.03796775623713589</v>
       </c>
       <c r="X778">
         <v>0.01160873533233175</v>
@@ -52984,7 +52984,7 @@
         <v>-0.03760090788191051</v>
       </c>
       <c r="N781">
-        <v>-0.03251023329800573</v>
+        <v>-0.03251023329800584</v>
       </c>
       <c r="O781">
         <v>-0.05419303633383743</v>
@@ -53247,7 +53247,7 @@
         <v>-0.04548898800211887</v>
       </c>
       <c r="C785">
-        <v>-0.04459304256069041</v>
+        <v>-0.0445930425606903</v>
       </c>
       <c r="D785">
         <v>-0.04171315774382756</v>
@@ -53265,7 +53265,7 @@
         <v>-0.04770311946470429</v>
       </c>
       <c r="I785">
-        <v>-0.03692917539547758</v>
+        <v>-0.03692917539547746</v>
       </c>
       <c r="J785">
         <v>-0.03631546020216214</v>
@@ -53372,7 +53372,7 @@
         <v>0.03499072625530086</v>
       </c>
       <c r="T786">
-        <v>-0.05374536248020545</v>
+        <v>-0.05374536248020556</v>
       </c>
       <c r="U786">
         <v>0.01944158664190843</v>
@@ -53854,7 +53854,7 @@
         <v>0.01220878423491811</v>
       </c>
       <c r="H793">
-        <v>-0.02411381480018049</v>
+        <v>-0.0241138148001806</v>
       </c>
       <c r="I793">
         <v>-0.003650794574132421</v>
@@ -54307,7 +54307,7 @@
         <v>0.008740184773826876</v>
       </c>
       <c r="K799">
-        <v>0.01407273624142946</v>
+        <v>0.01407273624142968</v>
       </c>
       <c r="L799">
         <v>0.003803598137904318</v>
@@ -54343,7 +54343,7 @@
         <v>-0.002516066997931943</v>
       </c>
       <c r="W799">
-        <v>-0.03168528729280451</v>
+        <v>-0.03168528729280462</v>
       </c>
       <c r="X799">
         <v>-0.009932163272825534</v>
@@ -54582,7 +54582,7 @@
         <v>0.0009604251691948118</v>
       </c>
       <c r="D803">
-        <v>0.001595879222806129</v>
+        <v>0.001595879222805907</v>
       </c>
       <c r="E803">
         <v>0.005954675594177505</v>
@@ -54603,7 +54603,7 @@
         <v>0.01231883675114887</v>
       </c>
       <c r="K803">
-        <v>-0.001055620153539216</v>
+        <v>-0.001055620153539105</v>
       </c>
       <c r="L803">
         <v>-0.01354041814147577</v>
@@ -54659,7 +54659,7 @@
         <v>-0.008195596218029455</v>
       </c>
       <c r="E804">
-        <v>0.008955871409461302</v>
+        <v>0.008955871409461524</v>
       </c>
       <c r="F804">
         <v>0.02446468765317289</v>
@@ -54819,7 +54819,7 @@
         <v>0.00502802854711204</v>
       </c>
       <c r="I806">
-        <v>0.01161589722151546</v>
+        <v>0.01161589722151524</v>
       </c>
       <c r="J806">
         <v>0.02066099837418012</v>
@@ -55840,7 +55840,7 @@
         <v>0.03068755265968148</v>
       </c>
       <c r="D820">
-        <v>0.01257851107943875</v>
+        <v>0.01257851107943853</v>
       </c>
       <c r="E820">
         <v>0.01723644901560051</v>
@@ -56110,7 +56110,7 @@
         <v>0.06868278069138056</v>
       </c>
       <c r="T823">
-        <v>-0.03774770031809127</v>
+        <v>-0.03774770031809138</v>
       </c>
       <c r="U823">
         <v>0.02630634622710004</v>
@@ -56169,7 +56169,7 @@
         <v>0.004837347996976327</v>
       </c>
       <c r="O824">
-        <v>0.0161547337707868</v>
+        <v>0.01615473377078702</v>
       </c>
       <c r="P824">
         <v>0.04454520054922129</v>
@@ -56317,7 +56317,7 @@
         <v>-0.0104614131429217</v>
       </c>
       <c r="O826">
-        <v>0.02719544624516979</v>
+        <v>0.02719544624517001</v>
       </c>
       <c r="P826">
         <v>0.006061974681928595</v>
@@ -56746,7 +56746,7 @@
         <v>0.005054415149464475</v>
       </c>
       <c r="J832">
-        <v>0.000892582981392831</v>
+        <v>0.000892582981393053</v>
       </c>
       <c r="K832">
         <v>0.04558961519271421</v>
@@ -57060,13 +57060,13 @@
         <v>-0.0005665549996618502</v>
       </c>
       <c r="P836">
-        <v>-0.01739475394381462</v>
+        <v>-0.01739475394381473</v>
       </c>
       <c r="Q836">
         <v>-0.01015995047892437</v>
       </c>
       <c r="R836">
-        <v>-0.02270561084156619</v>
+        <v>-0.02270561084156608</v>
       </c>
       <c r="S836">
         <v>-0.02677437726759191</v>
@@ -57101,7 +57101,7 @@
         <v>-0.06960234787897701</v>
       </c>
       <c r="E837">
-        <v>-0.1015065683450728</v>
+        <v>-0.1015065683450727</v>
       </c>
       <c r="F837">
         <v>-0.09685172560827537</v>
@@ -57320,7 +57320,7 @@
         <v>0.01061311910469764</v>
       </c>
       <c r="D840">
-        <v>0.01752602170291806</v>
+        <v>0.01752602170291784</v>
       </c>
       <c r="E840">
         <v>0.04477678179062794</v>
@@ -57480,7 +57480,7 @@
         <v>-0.05820318476273412</v>
       </c>
       <c r="H842">
-        <v>-0.04123628362933396</v>
+        <v>-0.04123628362933385</v>
       </c>
       <c r="I842">
         <v>-0.01149123809714825</v>
@@ -58081,7 +58081,7 @@
         <v>-0.05969224829261599</v>
       </c>
       <c r="K850">
-        <v>-0.06972141657120656</v>
+        <v>-0.06972141657120667</v>
       </c>
       <c r="L850">
         <v>-0.0426908982137375</v>
@@ -58306,7 +58306,7 @@
         <v>-0.01778165487523531</v>
       </c>
       <c r="L853">
-        <v>-0.009802778032910298</v>
+        <v>-0.00980277803291052</v>
       </c>
       <c r="M853">
         <v>-0.01094253532376033</v>
@@ -58362,7 +58362,7 @@
         <v>-0.02531779133863155</v>
       </c>
       <c r="F854">
-        <v>-0.03090770494275397</v>
+        <v>-0.03090770494275408</v>
       </c>
       <c r="G854">
         <v>-0.04040542817390602</v>
@@ -58821,7 +58821,7 @@
         <v>-0.02835411920123254</v>
       </c>
       <c r="K860">
-        <v>-0.009004840818474968</v>
+        <v>-0.009004840818475079</v>
       </c>
       <c r="L860">
         <v>0.004513717939313322</v>
@@ -58957,7 +58957,7 @@
         <v>0.007692244134258397</v>
       </c>
       <c r="G862">
-        <v>0.04640235523454384</v>
+        <v>0.04640235523454361</v>
       </c>
       <c r="H862">
         <v>-0.003198777570923017</v>
@@ -59253,7 +59253,7 @@
         <v>0.007649448940465486</v>
       </c>
       <c r="G866">
-        <v>-0.007470848098316774</v>
+        <v>-0.007470848098316996</v>
       </c>
       <c r="H866">
         <v>0.006273165389755864</v>
@@ -59952,7 +59952,7 @@
         <v>0.043778449558461</v>
       </c>
       <c r="R875">
-        <v>0.03729077273358716</v>
+        <v>0.03729077273358694</v>
       </c>
       <c r="S875">
         <v>0.03533600097194523</v>
@@ -60097,7 +60097,7 @@
         <v>-0.002305213138665274</v>
       </c>
       <c r="Q877">
-        <v>-0.01072156477039321</v>
+        <v>-0.01072156477039332</v>
       </c>
       <c r="R877">
         <v>-0.01163521838536286</v>
@@ -60653,7 +60653,7 @@
         <v>0.04079968412679502</v>
       </c>
       <c r="E885">
-        <v>0.04767298048143553</v>
+        <v>0.04767298048143531</v>
       </c>
       <c r="F885">
         <v>0.08761243168884891</v>
@@ -60801,7 +60801,7 @@
         <v>0.008891990891393586</v>
       </c>
       <c r="E887">
-        <v>0.02484052288077976</v>
+        <v>0.02484052288077998</v>
       </c>
       <c r="F887">
         <v>-0.002648876143718448</v>
@@ -61023,7 +61023,7 @@
         <v>0.007601900493213076</v>
       </c>
       <c r="E890">
-        <v>0.006736001811592729</v>
+        <v>0.006736001811592951</v>
       </c>
       <c r="F890">
         <v>0.01455057909779334</v>
@@ -61127,7 +61127,7 @@
         <v>-0.02306319300769311</v>
       </c>
       <c r="O891">
-        <v>0.003048541988760922</v>
+        <v>0.0030485419887607</v>
       </c>
       <c r="P891">
         <v>-0.005327886141087812</v>
@@ -61263,7 +61263,7 @@
         <v>0.01688175731097563</v>
       </c>
       <c r="K893">
-        <v>0.01786952987167134</v>
+        <v>0.01786952987167156</v>
       </c>
       <c r="L893">
         <v>-0.004190969984273374</v>
@@ -61840,7 +61840,7 @@
         <v>0.006300401348867224</v>
       </c>
       <c r="F901">
-        <v>0.02032873773486354</v>
+        <v>0.0203287377348631</v>
       </c>
       <c r="G901">
         <v>0.03013545486980429</v>
@@ -62373,7 +62373,7 @@
         <v>-0.03334591678174248</v>
       </c>
       <c r="K908">
-        <v>-0.02176497141551115</v>
+        <v>-0.02176497141551126</v>
       </c>
       <c r="L908">
         <v>0.00281114559014628</v>
@@ -62687,7 +62687,7 @@
         <v>0.01656009050323659</v>
       </c>
       <c r="Q912">
-        <v>0.0107662300369189</v>
+        <v>0.01076623003691868</v>
       </c>
       <c r="R912">
         <v>0.01832650169401573</v>
@@ -62725,7 +62725,7 @@
         <v>-0.02869753807194553</v>
       </c>
       <c r="E913">
-        <v>0.007890533847088488</v>
+        <v>0.00789053384708871</v>
       </c>
       <c r="F913">
         <v>-0.02603503922505201</v>
@@ -63175,7 +63175,7 @@
         <v>0.03911715958411177</v>
       </c>
       <c r="G919">
-        <v>0.02779227278846874</v>
+        <v>0.02779227278846852</v>
       </c>
       <c r="H919">
         <v>0.00160822290488527</v>
@@ -63308,7 +63308,7 @@
         <v>42967</v>
       </c>
       <c r="B921">
-        <v>-0.010885848805958</v>
+        <v>-0.01088584880595822</v>
       </c>
       <c r="C921">
         <v>-0.007340959652547108</v>
@@ -64128,7 +64128,7 @@
         <v>0.003401736461661642</v>
       </c>
       <c r="D932">
-        <v>0.003858186925452367</v>
+        <v>0.003858186925452145</v>
       </c>
       <c r="E932">
         <v>-0.003537530418858847</v>
@@ -64347,7 +64347,7 @@
         <v>0.006826129853755525</v>
       </c>
       <c r="C935">
-        <v>-0.00218266210104523</v>
+        <v>-0.002182662101045341</v>
       </c>
       <c r="D935">
         <v>-0.0009635590855813225</v>
@@ -64623,7 +64623,7 @@
         <v>0.02715922679406568</v>
       </c>
       <c r="U938">
-        <v>0.02155503764470978</v>
+        <v>0.02155503764470956</v>
       </c>
       <c r="V938">
         <v>0.03196313583327592</v>
@@ -64996,7 +64996,7 @@
         <v>0.01136497822780647</v>
       </c>
       <c r="V943">
-        <v>0.004463483597869855</v>
+        <v>0.004463483597869633</v>
       </c>
       <c r="W943">
         <v>-0.01991515295563384</v>
@@ -65457,7 +65457,7 @@
         <v>0.04951124476580215</v>
       </c>
       <c r="C950">
-        <v>0.03188676422919978</v>
+        <v>0.0318867642292</v>
       </c>
       <c r="D950">
         <v>0.03501182297265837</v>
@@ -65564,7 +65564,7 @@
         <v>-0.0008971355382361157</v>
       </c>
       <c r="N951">
-        <v>0.0002717655888091475</v>
+        <v>0.0002717655888089254</v>
       </c>
       <c r="O951">
         <v>0.01845669598889565</v>
@@ -65644,7 +65644,7 @@
         <v>-0.04059562764051838</v>
       </c>
       <c r="P952">
-        <v>-0.02968576829487946</v>
+        <v>-0.02968576829487957</v>
       </c>
       <c r="Q952">
         <v>0.00385941252082711</v>
@@ -65703,7 +65703,7 @@
         <v>0.02691129531919745</v>
       </c>
       <c r="K953">
-        <v>0.03629642642376263</v>
+        <v>0.03629642642376285</v>
       </c>
       <c r="L953">
         <v>0.007821547239239557</v>
@@ -66286,7 +66286,7 @@
         <v>-0.02172655499269271</v>
       </c>
       <c r="H961">
-        <v>-0.02563085773761253</v>
+        <v>-0.02563085773761242</v>
       </c>
       <c r="I961">
         <v>0.02234584199371836</v>
@@ -66390,7 +66390,7 @@
         <v>0.02244336673133063</v>
       </c>
       <c r="R962">
-        <v>0.01358614614819253</v>
+        <v>0.01358614614819276</v>
       </c>
       <c r="S962">
         <v>0.03539863186281145</v>
@@ -66505,7 +66505,7 @@
         <v>-0.02432620949558062</v>
       </c>
       <c r="G964">
-        <v>-0.03110834273138174</v>
+        <v>-0.03110834273138163</v>
       </c>
       <c r="H964">
         <v>-0.01528711577056696</v>
@@ -66585,7 +66585,7 @@
         <v>0.003815518769669568</v>
       </c>
       <c r="I965">
-        <v>-0.01891570791945685</v>
+        <v>-0.01891570791945674</v>
       </c>
       <c r="J965">
         <v>-0.02543942678010169</v>
@@ -66902,7 +66902,7 @@
         <v>-0.005883359120223086</v>
       </c>
       <c r="P969">
-        <v>-0.02292592525265857</v>
+        <v>-0.02292592525265869</v>
       </c>
       <c r="Q969">
         <v>-0.006713809989665531</v>
@@ -67310,7 +67310,7 @@
         <v>0.004268397008645897</v>
       </c>
       <c r="D975">
-        <v>0.001851752120146211</v>
+        <v>0.001851752120146433</v>
       </c>
       <c r="E975">
         <v>-0.0008730236212906028</v>
@@ -67378,7 +67378,7 @@
         <v>43352</v>
       </c>
       <c r="B976">
-        <v>0.0138790319594968</v>
+        <v>0.01387903195949658</v>
       </c>
       <c r="C976">
         <v>-0.00404061673600653</v>
@@ -68758,7 +68758,7 @@
         <v>-0.0001658453585763331</v>
       </c>
       <c r="R994">
-        <v>0.01552009977862223</v>
+        <v>0.01552009977862201</v>
       </c>
       <c r="S994">
         <v>0.005246769599719814</v>
@@ -68900,7 +68900,7 @@
         <v>-0.03848675150375502</v>
       </c>
       <c r="P996">
-        <v>-0.01739943278491474</v>
+        <v>-0.01739943278491463</v>
       </c>
       <c r="Q996">
         <v>-0.0311120033375295</v>
@@ -69681,7 +69681,7 @@
         <v>0.01046249895442397</v>
       </c>
       <c r="E1007">
-        <v>0.05602542150140422</v>
+        <v>0.05602542150140399</v>
       </c>
       <c r="F1007">
         <v>0.03748358452516731</v>
@@ -70102,7 +70102,7 @@
         <v>0.000977159908641223</v>
       </c>
       <c r="V1012">
-        <v>0.01107229995597292</v>
+        <v>0.01107229995597314</v>
       </c>
       <c r="W1012">
         <v>-0.04735929429607033</v>
@@ -70238,7 +70238,7 @@
         <v>-0.02353896584795578</v>
       </c>
       <c r="R1014">
-        <v>-0.040941578741024</v>
+        <v>-0.04094157874102411</v>
       </c>
       <c r="S1014">
         <v>-0.02490375148115032</v>
@@ -70273,13 +70273,13 @@
         <v>0.04920290033519437</v>
       </c>
       <c r="E1015">
-        <v>0.03020065477827494</v>
+        <v>0.03020065477827472</v>
       </c>
       <c r="F1015">
         <v>0.04053189481269404</v>
       </c>
       <c r="G1015">
-        <v>0.05695842983551591</v>
+        <v>0.05695842983551569</v>
       </c>
       <c r="H1015">
         <v>0.03353354708108114</v>
@@ -70371,7 +70371,7 @@
         <v>-0.01688360284589163</v>
       </c>
       <c r="M1016">
-        <v>0.01111586505779094</v>
+        <v>0.01111586505779072</v>
       </c>
       <c r="N1016">
         <v>-0.003726485407995472</v>
@@ -70501,7 +70501,7 @@
         <v>0.03129329570152195</v>
       </c>
       <c r="G1018">
-        <v>0.03030671257857254</v>
+        <v>0.03030671257857231</v>
       </c>
       <c r="H1018">
         <v>-0.001382372491680939</v>
@@ -70732,7 +70732,7 @@
         <v>-0.02808283912740794</v>
       </c>
       <c r="J1021">
-        <v>-0.001963250020813545</v>
+        <v>-0.001963250020813656</v>
       </c>
       <c r="K1021">
         <v>-0.01069717316056418</v>
@@ -70969,7 +70969,7 @@
         <v>-0.04342172844466075</v>
       </c>
       <c r="O1024">
-        <v>0.01243003658714703</v>
+        <v>0.01243003658714725</v>
       </c>
       <c r="P1024">
         <v>-0.01268327503161337</v>
@@ -70984,7 +70984,7 @@
         <v>-0.02757617929208256</v>
       </c>
       <c r="T1024">
-        <v>-0.01107789909607637</v>
+        <v>-0.01107789909607659</v>
       </c>
       <c r="U1024">
         <v>-0.006201977075135034</v>
@@ -71534,7 +71534,7 @@
         <v>-0.01852269857187472</v>
       </c>
       <c r="F1032">
-        <v>-0.03339053794763791</v>
+        <v>-0.03339053794763802</v>
       </c>
       <c r="G1032">
         <v>-0.01842890320387391</v>
@@ -71567,7 +71567,7 @@
         <v>-0.03511466884278747</v>
       </c>
       <c r="Q1032">
-        <v>-0.0306203196295517</v>
+        <v>-0.03062031962955147</v>
       </c>
       <c r="R1032">
         <v>-0.0400504906530309</v>
@@ -71679,7 +71679,7 @@
         <v>0.02992424974474339</v>
       </c>
       <c r="E1034">
-        <v>0.03805756625272427</v>
+        <v>0.03805756625272405</v>
       </c>
       <c r="F1034">
         <v>0.04980976082074728</v>
@@ -72621,7 +72621,7 @@
         <v>0.01714755032956949</v>
       </c>
       <c r="W1046">
-        <v>0.03147385638408662</v>
+        <v>0.0314738563840864</v>
       </c>
       <c r="X1046">
         <v>0.009427897386729667</v>
@@ -72641,7 +72641,7 @@
         <v>-0.02329285009278814</v>
       </c>
       <c r="E1047">
-        <v>0.01565372224196615</v>
+        <v>0.01565372224196637</v>
       </c>
       <c r="F1047">
         <v>-0.0008636746855901212</v>
@@ -73165,7 +73165,7 @@
         <v>-0.09183128270040686</v>
       </c>
       <c r="G1054">
-        <v>-0.03435273953646567</v>
+        <v>-0.03435273953646589</v>
       </c>
       <c r="H1054">
         <v>-0.02390261331821797</v>
@@ -73245,7 +73245,7 @@
         <v>-0.1096430082319629</v>
       </c>
       <c r="I1055">
-        <v>-0.1671603661454665</v>
+        <v>-0.1671603661454663</v>
       </c>
       <c r="J1055">
         <v>-0.08130669381709166</v>
@@ -73281,7 +73281,7 @@
         <v>-0.03826651616717236</v>
       </c>
       <c r="U1055">
-        <v>-0.06287466658794305</v>
+        <v>-0.06287466658794294</v>
       </c>
       <c r="V1055">
         <v>-0.01695873750357824</v>
@@ -73301,7 +73301,7 @@
         <v>-0.1780804486621409</v>
       </c>
       <c r="C1056">
-        <v>-0.1634885022650778</v>
+        <v>-0.1634885022650776</v>
       </c>
       <c r="D1056">
         <v>-0.1221007620135908</v>
@@ -73331,7 +73331,7 @@
         <v>-0.03645549692118855</v>
       </c>
       <c r="M1056">
-        <v>-0.1072300024892756</v>
+        <v>-0.1072300024892758</v>
       </c>
       <c r="N1056">
         <v>-0.1131154502572584</v>
@@ -73411,7 +73411,7 @@
         <v>0.0651489423864926</v>
       </c>
       <c r="O1057">
-        <v>0.005184725750534636</v>
+        <v>0.005184725750534858</v>
       </c>
       <c r="P1057">
         <v>0.1285896529950914</v>
@@ -73449,7 +73449,7 @@
         <v>-0.006800230978663557</v>
       </c>
       <c r="C1058">
-        <v>-0.1492065218161086</v>
+        <v>-0.1492065218161087</v>
       </c>
       <c r="D1058">
         <v>-0.1178301986488237</v>
@@ -73458,7 +73458,7 @@
         <v>-0.06781490051007399</v>
       </c>
       <c r="F1058">
-        <v>-0.07268604664091471</v>
+        <v>-0.07268604664091483</v>
       </c>
       <c r="G1058">
         <v>-0.144065023325438</v>
@@ -73467,7 +73467,7 @@
         <v>-0.01712463488652438</v>
       </c>
       <c r="I1058">
-        <v>-0.1337506778267381</v>
+        <v>-0.1337506778267382</v>
       </c>
       <c r="J1058">
         <v>-0.07205934292480987</v>
@@ -73574,7 +73574,7 @@
         <v>0.007281694035741859</v>
       </c>
       <c r="T1059">
-        <v>0.1101032656256102</v>
+        <v>0.1101032656256105</v>
       </c>
       <c r="U1059">
         <v>0.1042102955367392</v>
@@ -73609,7 +73609,7 @@
         <v>-0.06355573466176367</v>
       </c>
       <c r="G1060">
-        <v>-0.04134166753832325</v>
+        <v>-0.04134166753832336</v>
       </c>
       <c r="H1060">
         <v>-0.01236027557820008</v>
@@ -73793,7 +73793,7 @@
         <v>0.02792754762691141</v>
       </c>
       <c r="S1062">
-        <v>-0.02394200479257347</v>
+        <v>-0.02394200479257325</v>
       </c>
       <c r="T1062">
         <v>0.02155772252071042</v>
@@ -73808,7 +73808,7 @@
         <v>-0.04834751496238565</v>
       </c>
       <c r="X1062">
-        <v>-0.002124810706405356</v>
+        <v>-0.002124810706405467</v>
       </c>
     </row>
     <row r="1063" spans="1:24">
@@ -73849,7 +73849,7 @@
         <v>0.01384432728977458</v>
       </c>
       <c r="M1063">
-        <v>0.002765563138988902</v>
+        <v>0.002765563138989124</v>
       </c>
       <c r="N1063">
         <v>-0.0009908929617959972</v>
@@ -74130,7 +74130,7 @@
         <v>0.2285538792435466</v>
       </c>
       <c r="H1067">
-        <v>0.1090217998121814</v>
+        <v>0.1090217998121812</v>
       </c>
       <c r="I1067">
         <v>0.1964488062391618</v>
@@ -74186,7 +74186,7 @@
         <v>43996</v>
       </c>
       <c r="B1068">
-        <v>-0.1116484983633788</v>
+        <v>-0.1116484983633789</v>
       </c>
       <c r="C1068">
         <v>-0.1348903802405771</v>
@@ -74195,13 +74195,13 @@
         <v>-0.1147033355339231</v>
       </c>
       <c r="E1068">
-        <v>-0.1021301081271835</v>
+        <v>-0.1021301081271836</v>
       </c>
       <c r="F1068">
         <v>-0.1184631218592824</v>
       </c>
       <c r="G1068">
-        <v>-0.1122994985464931</v>
+        <v>-0.1122994985464932</v>
       </c>
       <c r="H1068">
         <v>-0.06423733632060369</v>
@@ -74337,7 +74337,7 @@
         <v>-0.06350371280126321</v>
       </c>
       <c r="C1070">
-        <v>-0.06744868315909658</v>
+        <v>-0.06744868315909647</v>
       </c>
       <c r="D1070">
         <v>-0.07229330239981269</v>

</xml_diff>